<commit_message>
WebForm User Assignment execution
</commit_message>
<xml_diff>
--- a/testData/WebForm/TC012_WF_RRUserYN_OneConditionN_Test.xlsx
+++ b/testData/WebForm/TC012_WF_RRUserYN_OneConditionN_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="108">
   <si>
     <t>BuildUrl</t>
   </si>
@@ -316,6 +316,33 @@
   </si>
   <si>
     <t>9840027367</t>
+  </si>
+  <si>
+    <t>9840021629</t>
+  </si>
+  <si>
+    <t>9840073816</t>
+  </si>
+  <si>
+    <t>9840015053</t>
+  </si>
+  <si>
+    <t>9840007094</t>
+  </si>
+  <si>
+    <t>9840006017</t>
+  </si>
+  <si>
+    <t>9840015663</t>
+  </si>
+  <si>
+    <t>9840025646</t>
+  </si>
+  <si>
+    <t>9840041532</t>
+  </si>
+  <si>
+    <t>9840060976</t>
   </si>
 </sst>
 </file>
@@ -909,7 +936,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -1011,7 +1038,7 @@
         <v>61</v>
       </c>
       <c r="AN2" t="s" s="0">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="AO2" t="s" s="0">
         <v>78</v>
@@ -1079,7 +1106,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
@@ -1126,7 +1153,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
@@ -1173,7 +1200,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>11</v>
@@ -1221,7 +1248,7 @@
         <v>16</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>11</v>
@@ -1268,7 +1295,7 @@
         <v>16</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>11</v>
@@ -1315,7 +1342,7 @@
         <v>16</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>11</v>
@@ -1362,7 +1389,7 @@
         <v>16</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>11</v>
@@ -1409,7 +1436,7 @@
         <v>16</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>11</v>

</xml_diff>